<commit_message>
[EPMFARMATS-18154] Search function automation
</commit_message>
<xml_diff>
--- a/Application.Test/Test Cases/Test_Cases_Table_search_module_.xlsx
+++ b/Application.Test/Test Cases/Test_Cases_Table_search_module_.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t xml:space="preserve">Title </t>
   </si>
@@ -427,7 +427,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Valid Artist Name:
+      <t xml:space="preserve">Valid Song Name:
 </t>
     </r>
     <r>
@@ -465,12 +465,12 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"Divide" , "Encore"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Valid Song Name:
+      <t>"Shape of You" , "Mockingbird"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Valid Artist Name:
 </t>
     </r>
     <r>
@@ -508,12 +508,27 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"Shape of You" , "Mockingbird"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Valid Artist Name:
+      <t>"Ed Sheeran" , "Eminem"</t>
+    </r>
+  </si>
+  <si>
+    <t>Filter search results ("Songs" category)</t>
+  </si>
+  <si>
+    <t>Filter search results ("Artists" category)</t>
+  </si>
+  <si>
+    <t>Filter search results ("Albums" category)</t>
+  </si>
+  <si>
+    <t>Filter search results ("Playlists" category)</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Valid Album Name:
 </t>
     </r>
     <r>
@@ -551,7 +566,177 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"Ed Sheeran" , "Eminem"</t>
+      <t>"Divide" , "Encore"</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Enter the Playlist title in the search bar.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Valid Playlist Name:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-using valid characters
+-should not contain any special or undefined characters
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Example:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Eminem Top 10" , "Twenty One Pilots Mix"</t>
+    </r>
+  </si>
+  <si>
+    <t>3. Apply "Playlists" filter option.</t>
+  </si>
+  <si>
+    <t>3. Apply "Songs" filter option.</t>
+  </si>
+  <si>
+    <t>3. Apply "Artists" filter option.</t>
+  </si>
+  <si>
+    <t>3. Apply "Albums" filter option.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">After applying the filter:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Songs" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tab, displays a list of songs ranked by how closely their names match your search input.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">After applying the filter:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Artist" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tab, displays a grid of artists ranked by how closely their names match your search input.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">After applying the filter:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Albums" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tab, displays a grid of albums ranked by how closely their names match your search input.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">After applying the filter:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Playlists" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tab, displays a grid of playlists ranked by how closely their names match your search input.</t>
     </r>
   </si>
 </sst>
@@ -633,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -646,13 +831,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -934,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -972,10 +1166,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2"/>
@@ -987,10 +1181,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="7" t="s">
-        <v>24</v>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -1000,10 +1194,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2"/>
@@ -1015,10 +1209,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="7" t="s">
-        <v>25</v>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
@@ -1028,10 +1222,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2"/>
@@ -1043,10 +1237,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="7" t="s">
-        <v>23</v>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -1056,10 +1250,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2"/>
@@ -1071,9 +1265,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="7" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1086,19 +1280,202 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="19" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="10"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="10"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="10"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" ht="150" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="18">
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B2:B3"/>
@@ -1107,6 +1484,16 @@
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A19:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>